<commit_message>
Fix MLCLSP batch model
</commit_message>
<xml_diff>
--- a/szablony/MLCLSP_PARTIE_wejscie.xlsx
+++ b/szablony/MLCLSP_PARTIE_wejscie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\STUDIA\MAGISTERKA\Python\WPy64-3771\notebooks\magisterka\szablony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC92ED3-EFCA-4521-8231-AF7252F47610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E4E4D-36FF-45C4-A6AF-16DAA3D6537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
         <t>[Komentarz podzielony na wątki]
 Używana wersja programu Excel umożliwia odczytanie tego komentarza podzielonego na wątki, jednak wszelkie wprowadzone w nim zmiany zostaną usunięte po otwarciu pliku w nowszej wersji programu Excel. Dowiedz się więcej: https://go.microsoft.com/fwlink/?linkid=870924
 Komentarz:
-    Macierz określa czas przezbrojenia maszyny m na produkcję wyrobu i. Wyroby określone są w pierwszej kolumnie natomiast maszyny w pierwszym wierszu. Wartość 0 oznacza brak możliwości produkcji wyrobu i na danej maszynie m.</t>
+    Macierz określa czas przezbrojenia z wyrobu i na produkcję wyrobu j. Wyroby i określone są w pierwszej kolumnie natomiast wyroby j w pierwszym wierszu. Wartość 0 oznacza brak możliwości produkcji wyrobu i na danej maszynie m.</t>
       </text>
     </comment>
   </commentList>
@@ -497,7 +497,7 @@
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="A1" dT="2023-02-05T13:38:29.08" personId="{A46F1C30-488C-4073-8F24-2BD2360DCB2A}" id="{8495A521-7FE0-4C8F-9F81-F9356F768487}">
-    <text>Macierz określa czas przezbrojenia maszyny m na produkcję wyrobu i. Wyroby określone są w pierwszej kolumnie natomiast maszyny w pierwszym wierszu. Wartość 0 oznacza brak możliwości produkcji wyrobu i na danej maszynie m.</text>
+    <text>Macierz określa czas przezbrojenia z wyrobu i na produkcję wyrobu j. Wyroby i określone są w pierwszej kolumnie natomiast wyroby j w pierwszym wierszu. Wartość 0 oznacza brak możliwości produkcji wyrobu i na danej maszynie m.</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -757,7 +757,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{880ACAF4-18D6-49D3-B2EA-96217C18902E}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -841,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F799A6C2-5E4D-434D-A9EE-3D27429D4330}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,7 +945,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Prepare models for simulation possibility
</commit_message>
<xml_diff>
--- a/szablony/MLCLSP_PARTIE_wejscie.xlsx
+++ b/szablony/MLCLSP_PARTIE_wejscie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\STUDIA\MAGISTERKA\Python\WPy64-3771\notebooks\magisterka\szablony\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E4E4D-36FF-45C4-A6AF-16DAA3D6537E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5442FAD-CB47-4CAE-B7A2-7A6BA45A8ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WYROBY" sheetId="2" r:id="rId1"/>
@@ -515,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AD956B-9504-40BE-A25F-F196DD8FFA60}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB58457-BC35-4E0C-85B1-756A6961CF57}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>